<commit_message>
[UPDATE] Actualizados tags de excel
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel/plantilla.xlsx
+++ b/src/main/resources/templates/excel/plantilla.xlsx
@@ -51,7 +51,7 @@
     <t>&lt;bbva:money amount="${deliveryman.salary.amount}" currency="${deliveryman.salary.currency}"/&gt;&lt;/jt:forEach&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve"> ${deliveryman.time}</t>
+    <t xml:space="preserve"> &lt;bbva:localTime value="${deliveryman.time}"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="B1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>